<commit_message>
meto Reparaciones como modulo aparte de la aplicacion
</commit_message>
<xml_diff>
--- a/xls/380.xlsx
+++ b/xls/380.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Componentes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="459">
   <si>
     <t>Componente</t>
   </si>
@@ -843,18 +843,6 @@
     <t>Conformado</t>
   </si>
   <si>
-    <t>Instalaciones</t>
-  </si>
-  <si>
-    <t>Nevera</t>
-  </si>
-  <si>
-    <t>C.Produccion</t>
-  </si>
-  <si>
-    <t>Manteniniento</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -867,30 +855,15 @@
     <t>Desencolados</t>
   </si>
   <si>
-    <t>I.M.A</t>
-  </si>
-  <si>
-    <t>Roturas_de_Telas</t>
-  </si>
-  <si>
-    <t>F.V</t>
-  </si>
-  <si>
     <t>Abult._y_Depr.</t>
   </si>
   <si>
     <t>Marcas</t>
   </si>
   <si>
-    <t>Alturas</t>
-  </si>
-  <si>
     <t>Espesores</t>
   </si>
   <si>
-    <t>Contornos</t>
-  </si>
-  <si>
     <t>Arrugas</t>
   </si>
   <si>
@@ -903,87 +876,36 @@
     <t>Desp._Rigidiz.</t>
   </si>
   <si>
-    <t>Long._Rigidiz.</t>
-  </si>
-  <si>
     <t>Escalones</t>
   </si>
   <si>
-    <t>Irisaciones</t>
-  </si>
-  <si>
     <t>Repasos</t>
   </si>
   <si>
-    <t>Cosmética</t>
-  </si>
-  <si>
-    <t>Taladro</t>
-  </si>
-  <si>
     <t>Materiales</t>
   </si>
   <si>
     <t>Averías</t>
   </si>
   <si>
-    <t>Puesta_a_Punto</t>
-  </si>
-  <si>
     <t>Rotura_de_B.V.</t>
   </si>
   <si>
-    <t>Desp.Referenceuerzos</t>
-  </si>
-  <si>
     <t>Arreglos_Doc.</t>
   </si>
   <si>
     <t>Reposiciones</t>
   </si>
   <si>
-    <t>Deformaciones</t>
-  </si>
-  <si>
     <t>Holguras</t>
   </si>
   <si>
-    <t>Fab.Errónea</t>
-  </si>
-  <si>
-    <t>F.C.</t>
-  </si>
-  <si>
-    <t>Adhesivo</t>
-  </si>
-  <si>
-    <t>Desp.Omegas</t>
-  </si>
-  <si>
     <t>M.B.</t>
   </si>
   <si>
-    <t>T.Pendientes</t>
-  </si>
-  <si>
-    <t>Contaminacion</t>
-  </si>
-  <si>
     <t>Probetas</t>
   </si>
   <si>
-    <t>T.Externos</t>
-  </si>
-  <si>
-    <t>Rep.Erronea</t>
-  </si>
-  <si>
-    <t>Falta_de_Personal</t>
-  </si>
-  <si>
-    <t>Clav.Herramienta</t>
-  </si>
-  <si>
     <t>Acoplamiento</t>
   </si>
   <si>
@@ -1392,9 +1314,6 @@
     <t>25 DER 2</t>
   </si>
   <si>
-    <t>Programacion</t>
-  </si>
-  <si>
     <t>I.M.A.</t>
   </si>
   <si>
@@ -1416,15 +1335,6 @@
     <t>Desp. Rigidiz.</t>
   </si>
   <si>
-    <t>Long. Rigidiz.</t>
-  </si>
-  <si>
-    <t>Taladrado</t>
-  </si>
-  <si>
-    <t>Puesta a Punto</t>
-  </si>
-  <si>
     <t>Rotura de B.V.</t>
   </si>
   <si>
@@ -1434,22 +1344,73 @@
     <t>Contaminación</t>
   </si>
   <si>
-    <t>Rep.Errónea</t>
-  </si>
-  <si>
-    <t>Falta de personal</t>
-  </si>
-  <si>
-    <t>Clav.herramienta</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>LAYUP</t>
   </si>
   <si>
     <t>CONFORMADO</t>
+  </si>
+  <si>
+    <t>Fab. Errónea</t>
+  </si>
+  <si>
+    <t>Desp. Omegas</t>
+  </si>
+  <si>
+    <t>Rep. Errónea</t>
+  </si>
+  <si>
+    <t>T. Externos</t>
+  </si>
+  <si>
+    <t>Clav. Herramienta</t>
+  </si>
+  <si>
+    <t>Defectos superficiales</t>
+  </si>
+  <si>
+    <t>Dimensiones fuera de tolerancia</t>
+  </si>
+  <si>
+    <t>Falta de resina</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Clav._Herramienta</t>
+  </si>
+  <si>
+    <t>Defectos_superficiales</t>
+  </si>
+  <si>
+    <t>Desp._Omegas</t>
+  </si>
+  <si>
+    <t>Dimensiones_fuera_de_tolerancia</t>
+  </si>
+  <si>
+    <t>Fab._Errónea</t>
+  </si>
+  <si>
+    <t>Falta_de_resina</t>
+  </si>
+  <si>
+    <t>Rep._Errónea</t>
+  </si>
+  <si>
+    <t>Roturas_de_telas</t>
+  </si>
+  <si>
+    <t>T._Externos</t>
+  </si>
+  <si>
+    <t>C. Producción</t>
+  </si>
+  <si>
+    <t>Mantenimiento</t>
+  </si>
+  <si>
+    <t>Programación</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1840,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,7 +1809,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1856,7 +1817,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>322</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1864,7 +1825,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1872,7 +1833,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>327</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1880,7 +1841,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1888,7 +1849,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1896,7 +1857,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>328</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1904,7 +1865,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,23 +1873,23 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -1959,7 +1920,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1970,7 +1931,7 @@
         <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>374</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1981,7 +1942,7 @@
         <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>375</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1992,7 +1953,7 @@
         <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2003,7 +1964,7 @@
         <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,7 +1975,7 @@
         <v>111</v>
       </c>
       <c r="C6" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2025,7 +1986,7 @@
         <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2036,7 +1997,7 @@
         <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>380</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2047,7 +2008,7 @@
         <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>381</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2058,7 +2019,7 @@
         <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>382</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2069,7 +2030,7 @@
         <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>383</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2080,7 +2041,7 @@
         <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>384</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2091,7 +2052,7 @@
         <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>385</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2102,7 +2063,7 @@
         <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>386</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2113,7 +2074,7 @@
         <v>129</v>
       </c>
       <c r="C15" t="s">
-        <v>387</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2124,7 +2085,7 @@
         <v>131</v>
       </c>
       <c r="C16" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2135,7 +2096,7 @@
         <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2146,7 +2107,7 @@
         <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2157,7 +2118,7 @@
         <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>391</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2168,7 +2129,7 @@
         <v>139</v>
       </c>
       <c r="C20" t="s">
-        <v>392</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2179,7 +2140,7 @@
         <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>393</v>
+        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2190,7 +2151,7 @@
         <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2201,7 +2162,7 @@
         <v>145</v>
       </c>
       <c r="C23" t="s">
-        <v>395</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2212,7 +2173,7 @@
         <v>147</v>
       </c>
       <c r="C24" t="s">
-        <v>396</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2223,7 +2184,7 @@
         <v>149</v>
       </c>
       <c r="C25" t="s">
-        <v>397</v>
+        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2234,7 +2195,7 @@
         <v>151</v>
       </c>
       <c r="C26" t="s">
-        <v>398</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2245,7 +2206,7 @@
         <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>399</v>
+        <v>373</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2256,7 +2217,7 @@
         <v>155</v>
       </c>
       <c r="C28" t="s">
-        <v>400</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2267,7 +2228,7 @@
         <v>157</v>
       </c>
       <c r="C29" t="s">
-        <v>401</v>
+        <v>375</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2278,7 +2239,7 @@
         <v>159</v>
       </c>
       <c r="C30" t="s">
-        <v>402</v>
+        <v>376</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2289,7 +2250,7 @@
         <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>403</v>
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2300,7 +2261,7 @@
         <v>163</v>
       </c>
       <c r="C32" t="s">
-        <v>404</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2311,7 +2272,7 @@
         <v>165</v>
       </c>
       <c r="C33" t="s">
-        <v>405</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2322,7 +2283,7 @@
         <v>167</v>
       </c>
       <c r="C34" t="s">
-        <v>406</v>
+        <v>380</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2333,7 +2294,7 @@
         <v>169</v>
       </c>
       <c r="C35" t="s">
-        <v>407</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -2368,7 +2329,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,7 +2340,7 @@
         <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2390,7 +2351,7 @@
         <v>173</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2401,7 +2362,7 @@
         <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>438</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2412,7 +2373,7 @@
         <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>439</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2423,7 +2384,7 @@
         <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>422</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2434,7 +2395,7 @@
         <v>181</v>
       </c>
       <c r="C7" t="s">
-        <v>423</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2445,7 +2406,7 @@
         <v>183</v>
       </c>
       <c r="C8" t="s">
-        <v>440</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2456,7 +2417,7 @@
         <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>441</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2467,7 +2428,7 @@
         <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>424</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2478,7 +2439,7 @@
         <v>189</v>
       </c>
       <c r="C11" t="s">
-        <v>425</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2489,7 +2450,7 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>442</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,7 +2461,7 @@
         <v>193</v>
       </c>
       <c r="C13" t="s">
-        <v>443</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2511,7 +2472,7 @@
         <v>195</v>
       </c>
       <c r="C14" t="s">
-        <v>426</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2522,7 +2483,7 @@
         <v>197</v>
       </c>
       <c r="C15" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2533,7 +2494,7 @@
         <v>199</v>
       </c>
       <c r="C16" t="s">
-        <v>444</v>
+        <v>418</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2544,7 +2505,7 @@
         <v>201</v>
       </c>
       <c r="C17" t="s">
-        <v>445</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2555,7 +2516,7 @@
         <v>203</v>
       </c>
       <c r="C18" t="s">
-        <v>434</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2566,7 +2527,7 @@
         <v>205</v>
       </c>
       <c r="C19" t="s">
-        <v>446</v>
+        <v>420</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2577,7 +2538,7 @@
         <v>207</v>
       </c>
       <c r="C20" t="s">
-        <v>428</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2588,7 +2549,7 @@
         <v>209</v>
       </c>
       <c r="C21" t="s">
-        <v>429</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2599,7 +2560,7 @@
         <v>211</v>
       </c>
       <c r="C22" t="s">
-        <v>435</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2610,7 +2571,7 @@
         <v>213</v>
       </c>
       <c r="C23" t="s">
-        <v>447</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2621,7 +2582,7 @@
         <v>215</v>
       </c>
       <c r="C24" t="s">
-        <v>430</v>
+        <v>404</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2632,7 +2593,7 @@
         <v>217</v>
       </c>
       <c r="C25" t="s">
-        <v>431</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2643,7 +2604,7 @@
         <v>219</v>
       </c>
       <c r="C26" t="s">
-        <v>436</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2654,7 +2615,7 @@
         <v>221</v>
       </c>
       <c r="C27" t="s">
-        <v>448</v>
+        <v>422</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2665,7 +2626,7 @@
         <v>223</v>
       </c>
       <c r="C28" t="s">
-        <v>432</v>
+        <v>406</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2676,7 +2637,7 @@
         <v>225</v>
       </c>
       <c r="C29" t="s">
-        <v>433</v>
+        <v>407</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2687,7 +2648,7 @@
         <v>227</v>
       </c>
       <c r="C30" t="s">
-        <v>437</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2698,7 +2659,7 @@
         <v>229</v>
       </c>
       <c r="C31" t="s">
-        <v>449</v>
+        <v>423</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2709,7 +2670,7 @@
         <v>231</v>
       </c>
       <c r="C32" t="s">
-        <v>450</v>
+        <v>424</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2720,7 +2681,7 @@
         <v>233</v>
       </c>
       <c r="C33" t="s">
-        <v>451</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -2752,7 +2713,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2760,7 +2721,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>416</v>
+        <v>390</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2771,7 +2732,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>417</v>
+        <v>391</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2782,7 +2743,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>418</v>
+        <v>392</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2793,7 +2754,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>419</v>
+        <v>393</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2826,95 +2787,95 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
       <c r="B2" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
       <c r="C2" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
       <c r="B3" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
       <c r="C3" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>410</v>
+        <v>384</v>
       </c>
       <c r="B4" t="s">
-        <v>410</v>
+        <v>384</v>
       </c>
       <c r="C4" t="s">
-        <v>410</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>411</v>
+        <v>385</v>
       </c>
       <c r="B5" t="s">
-        <v>411</v>
+        <v>385</v>
       </c>
       <c r="C5" t="s">
-        <v>411</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>386</v>
       </c>
       <c r="B6" t="s">
-        <v>412</v>
+        <v>386</v>
       </c>
       <c r="C6" t="s">
-        <v>412</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>413</v>
+        <v>387</v>
       </c>
       <c r="B7" t="s">
-        <v>413</v>
+        <v>387</v>
       </c>
       <c r="C7" t="s">
-        <v>413</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>414</v>
+        <v>388</v>
       </c>
       <c r="B8" t="s">
-        <v>414</v>
+        <v>388</v>
       </c>
       <c r="C8" t="s">
-        <v>414</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
       <c r="B9" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
       <c r="C9" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -2980,7 +2941,7 @@
         <v>240</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>471</v>
+        <v>437</v>
       </c>
       <c r="O5" s="6"/>
     </row>
@@ -2989,7 +2950,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>470</v>
+        <v>436</v>
       </c>
       <c r="O6" s="6"/>
     </row>
@@ -3143,10 +3104,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja13"/>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3162,112 +3123,102 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>456</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>264</v>
+        <v>458</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>317</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -3283,383 +3234,311 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja14"/>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="11.28515625"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.28515625"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.28515625"/>
+    <col min="10" max="1025" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="B3" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B4" t="s">
-        <v>276</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B5" t="s">
-        <v>453</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B6" t="s">
-        <v>454</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>447</v>
       </c>
       <c r="B7" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>435</v>
       </c>
       <c r="B8" t="s">
-        <v>456</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>281</v>
+        <v>448</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B10" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B11" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B12" t="s">
-        <v>284</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>285</v>
+        <v>449</v>
       </c>
       <c r="B13" t="s">
-        <v>285</v>
+        <v>439</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B14" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>287</v>
+        <v>450</v>
       </c>
       <c r="B15" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B16" t="s">
-        <v>459</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B17" t="s">
-        <v>460</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>290</v>
+        <v>428</v>
       </c>
       <c r="B18" t="s">
-        <v>290</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>291</v>
+        <v>451</v>
       </c>
       <c r="B19" t="s">
-        <v>291</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="B20" t="s">
-        <v>292</v>
+        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>452</v>
       </c>
       <c r="B21" t="s">
-        <v>293</v>
+        <v>445</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B22" t="s">
-        <v>461</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>295</v>
+        <v>426</v>
       </c>
       <c r="B23" t="s">
-        <v>295</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B24" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="B25" t="s">
-        <v>462</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="B26" t="s">
-        <v>463</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="B27" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="B28" t="s">
-        <v>464</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>301</v>
+        <v>453</v>
       </c>
       <c r="B29" t="s">
-        <v>301</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="B30" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="B31" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="B32" t="s">
-        <v>304</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>305</v>
+        <v>454</v>
       </c>
       <c r="B33" t="s">
-        <v>305</v>
+        <v>427</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>306</v>
+        <v>446</v>
       </c>
       <c r="B34" t="s">
-        <v>306</v>
+        <v>446</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>307</v>
+        <v>455</v>
       </c>
       <c r="B35" t="s">
-        <v>307</v>
+        <v>441</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>308</v>
+        <v>261</v>
       </c>
       <c r="B36" t="s">
-        <v>308</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>309</v>
-      </c>
-      <c r="B37" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>310</v>
-      </c>
-      <c r="B38" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>311</v>
-      </c>
-      <c r="B39" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>312</v>
-      </c>
-      <c r="B40" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>313</v>
-      </c>
-      <c r="B41" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>314</v>
-      </c>
-      <c r="B42" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>315</v>
-      </c>
-      <c r="B43" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>316</v>
-      </c>
-      <c r="B44" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>261</v>
-      </c>
-      <c r="B45" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>318</v>
-      </c>
-      <c r="B46" t="s">
-        <v>469</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3677,7 +3556,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -3695,7 +3574,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3706,7 +3585,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3717,7 +3596,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3728,7 +3607,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3739,7 +3618,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3750,7 +3629,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>332</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3761,7 +3640,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3794,7 +3673,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3805,7 +3684,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3816,7 +3695,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3852,7 +3731,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3863,7 +3742,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3874,7 +3753,7 @@
         <v>33</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,7 +3764,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3896,7 +3775,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3927,7 +3806,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3938,7 +3817,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3949,7 +3828,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3960,7 +3839,7 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3971,7 +3850,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -4006,7 +3885,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4017,7 +3896,7 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4028,7 +3907,7 @@
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4039,7 +3918,7 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4050,7 +3929,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4095,7 +3974,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4106,7 +3985,7 @@
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4117,7 +3996,7 @@
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4128,7 +4007,7 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4139,7 +4018,7 @@
         <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>360</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4150,7 +4029,7 @@
         <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4161,7 +4040,7 @@
         <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>362</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4172,7 +4051,7 @@
         <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>363</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4183,7 +4062,7 @@
         <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4194,7 +4073,7 @@
         <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4205,7 +4084,7 @@
         <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>365</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4216,7 +4095,7 @@
         <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4263,7 +4142,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4274,7 +4153,7 @@
         <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>366</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4285,7 +4164,7 @@
         <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>368</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4296,7 +4175,7 @@
         <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4307,7 +4186,7 @@
         <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4318,7 +4197,7 @@
         <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>370</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4329,7 +4208,7 @@
         <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4340,7 +4219,7 @@
         <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4351,7 +4230,7 @@
         <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -4386,7 +4265,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4397,7 +4276,7 @@
         <v>95</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4408,7 +4287,7 @@
         <v>97</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>345</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4419,7 +4298,7 @@
         <v>99</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4430,7 +4309,7 @@
         <v>101</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>